<commit_message>
TableWrapper, preparation to Excel report. Not debugged.
</commit_message>
<xml_diff>
--- a/apricot-docs/ScanOutputPrototype.xlsx
+++ b/apricot-docs/ScanOutputPrototype.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AntonNazarov\git.apricot\apricot-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B64AAB-3062-4CDE-96DC-84E5AC11A209}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B1D950-05A4-4E8B-9968-F2E0F5E78044}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{6F7FA7A6-DD01-4D17-928F-3158747715F3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>payment_transaction</t>
   </si>
@@ -66,12 +66,6 @@
     <t>bit</t>
   </si>
   <si>
-    <t>PK</t>
-  </si>
-  <si>
-    <t>FK</t>
-  </si>
-  <si>
     <t>transaction_startdate_idx(transaction_started_date)</t>
   </si>
   <si>
@@ -85,6 +79,45 @@
   </si>
   <si>
     <t>child_table_2</t>
+  </si>
+  <si>
+    <t>IDX</t>
+  </si>
+  <si>
+    <t>UIDX</t>
+  </si>
+  <si>
+    <t>PK, FK</t>
+  </si>
+  <si>
+    <t>PARENT TABLES</t>
+  </si>
+  <si>
+    <t>CHILD TABLES</t>
+  </si>
+  <si>
+    <t>TABLES</t>
+  </si>
+  <si>
+    <t>pos</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Constraint</t>
+  </si>
+  <si>
+    <t>Column name, *mandatory</t>
+  </si>
+  <si>
+    <t>UC</t>
+  </si>
+  <si>
+    <t>FK1</t>
+  </si>
+  <si>
+    <t>PK- primary key, FK- foreign key, UC- unique constraint, IDX- index, UIDX- unique index</t>
   </si>
 </sst>
 </file>
@@ -116,7 +149,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -139,14 +172,143 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{680C23F6-A669-4485-B8FE-1DB1C531341B}">
-  <dimension ref="A2:F11"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,116 +635,170 @@
     <col min="2" max="2" width="6.85546875" customWidth="1"/>
     <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="11"/>
+      <c r="G2" s="12"/>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="2">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="2">
+        <v>7</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="1" t="s">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="2">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="2">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="2">
-        <v>6</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="2">
-        <v>7</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="B13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>16</v>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="16" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>